<commit_message>
First Draft of Results
</commit_message>
<xml_diff>
--- a/analysis/Exact Sobol.xlsx
+++ b/analysis/Exact Sobol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sin.1" sheetId="4" r:id="rId1"/>
@@ -611,19 +611,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -643,15 +643,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ard.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,7 +671,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rom.optimized.S1" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3870,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,19 +4017,19 @@
         <v>100</v>
       </c>
       <c r="D4" s="20">
-        <v>7.7136027250608197E-2</v>
+        <v>0.566785397777536</v>
       </c>
       <c r="E4" s="20">
-        <v>0.91420873079007703</v>
+        <v>0.244942064711416</v>
       </c>
       <c r="F4" s="20">
-        <v>-4.8621517384378298E-12</v>
+        <v>1.10824557633902E-3</v>
       </c>
       <c r="G4" s="20">
-        <v>-4.8621517384378298E-12</v>
+        <v>4.1212372945491903E-5</v>
       </c>
       <c r="H4" s="21">
-        <v>-4.8621517384378298E-12</v>
+        <v>2.2204973669157399E-2</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -4054,27 +4054,27 @@
       </c>
       <c r="Y4" s="20">
         <f t="array" ref="Y4:AC13">D4:H13-Y2:AC2</f>
-        <v>1.6643272506081941E-3</v>
+        <v>0.49131369777753597</v>
       </c>
       <c r="Z4" s="20">
-        <v>-1.0319269209922988E-2</v>
+        <v>-0.67958593528858402</v>
       </c>
       <c r="AA4" s="20">
-        <v>-4.8621517384378298E-12</v>
+        <v>1.10824557633902E-3</v>
       </c>
       <c r="AB4" s="20">
-        <v>-4.8621517384378298E-12</v>
+        <v>4.1212372945491903E-5</v>
       </c>
       <c r="AC4" s="21">
-        <v>-4.8621517384378298E-12</v>
+        <v>2.2204973669157399E-2</v>
       </c>
       <c r="AD4" s="25">
         <f t="array" ref="AD4">MAX(ABS(Y4:AC4))</f>
-        <v>1.0319269209922988E-2</v>
+        <v>0.67958593528858402</v>
       </c>
       <c r="AE4" s="25">
         <f t="array" ref="AE4">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y4:$AC4),0))</f>
-        <v>4.8621517384378298E-12</v>
+        <v>2.2204973669157399E-2</v>
       </c>
     </row>
     <row r="5" spans="1:40" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4085,19 +4085,19 @@
         <v>100</v>
       </c>
       <c r="D5" s="73">
-        <v>3.9532334089099001E-2</v>
+        <v>0.50100371618402195</v>
       </c>
       <c r="E5" s="73">
-        <v>0.45587626292574801</v>
+        <v>0.49193974231485799</v>
       </c>
       <c r="F5" s="73">
-        <v>2.15984203931216E-8</v>
+        <v>1.5163036689996099E-8</v>
       </c>
       <c r="G5" s="73">
-        <v>9.37338850435741E-10</v>
+        <v>5.3673180608491897E-8</v>
       </c>
       <c r="H5" s="74">
-        <v>0.48046600408589502</v>
+        <v>8.7624136953674297E-8</v>
       </c>
       <c r="I5" s="69"/>
       <c r="J5" s="69"/>
@@ -4120,27 +4120,27 @@
         <v>100</v>
       </c>
       <c r="Y5" s="73">
-        <v>-3.5939365910901001E-2</v>
+        <v>0.42553201618402192</v>
       </c>
       <c r="Z5" s="73">
-        <v>-0.46865173707425201</v>
+        <v>-0.43258825768514203</v>
       </c>
       <c r="AA5" s="73">
-        <v>2.15984203931216E-8</v>
+        <v>1.5163036689996099E-8</v>
       </c>
       <c r="AB5" s="73">
-        <v>9.37338850435741E-10</v>
+        <v>5.3673180608491897E-8</v>
       </c>
       <c r="AC5" s="74">
-        <v>0.48046600408589502</v>
+        <v>8.7624136953674297E-8</v>
       </c>
       <c r="AD5" s="75">
         <f t="array" ref="AD5">MAX(ABS(Y5:AC5))</f>
-        <v>0.48046600408589502</v>
+        <v>0.43258825768514203</v>
       </c>
       <c r="AE5" s="75">
         <f t="array" ref="AE5">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y5:$AC5),0))</f>
-        <v>0.48046600408589502</v>
+        <v>8.7624136953674297E-8</v>
       </c>
       <c r="AF5" s="13"/>
       <c r="AM5" s="13"/>
@@ -4154,19 +4154,19 @@
         <v>200</v>
       </c>
       <c r="D6" s="20">
-        <v>7.7794435976047904E-2</v>
+        <v>0.50387272716312204</v>
       </c>
       <c r="E6" s="20">
-        <v>0.919228082914468</v>
+        <v>0.49335407418464899</v>
       </c>
       <c r="F6" s="20">
-        <v>-1.30854879985109E-11</v>
+        <v>2.6698312198433301E-11</v>
       </c>
       <c r="G6" s="20">
-        <v>-1.30854879985109E-11</v>
+        <v>5.0461784545936602E-11</v>
       </c>
       <c r="H6" s="21">
-        <v>-1.30854879985109E-11</v>
+        <v>-1.23137940357182E-11</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4189,27 +4189,27 @@
         <v>200</v>
       </c>
       <c r="Y6" s="20">
-        <v>2.3227359760479016E-3</v>
+        <v>0.42840102716312201</v>
       </c>
       <c r="Z6" s="20">
-        <v>-5.2999170855320132E-3</v>
+        <v>-0.43117392581535102</v>
       </c>
       <c r="AA6" s="20">
-        <v>-1.30854879985109E-11</v>
+        <v>2.6698312198433301E-11</v>
       </c>
       <c r="AB6" s="20">
-        <v>-1.30854879985109E-11</v>
+        <v>5.0461784545936602E-11</v>
       </c>
       <c r="AC6" s="21">
-        <v>-1.30854879985109E-11</v>
+        <v>-1.23137940357182E-11</v>
       </c>
       <c r="AD6" s="25">
         <f t="array" ref="AD6">MAX(ABS(Y6:AC6))</f>
-        <v>5.2999170855320132E-3</v>
+        <v>0.43117392581535102</v>
       </c>
       <c r="AE6" s="25">
         <f t="array" ref="AE6">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y6:$AC6),0))</f>
-        <v>1.30854879985109E-11</v>
+        <v>5.0461784545936602E-11</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -4220,19 +4220,19 @@
         <v>200</v>
       </c>
       <c r="D7" s="20">
-        <v>7.6820447381556398E-2</v>
+        <v>0.46559513692375798</v>
       </c>
       <c r="E7" s="20">
-        <v>0.91791984040576902</v>
+        <v>0.46453198345819402</v>
       </c>
       <c r="F7" s="20">
-        <v>2.7937661256342299E-8</v>
+        <v>2.0410107431561801E-5</v>
       </c>
       <c r="G7" s="20">
-        <v>-1.33461790304268E-8</v>
+        <v>-3.9342847907073503E-5</v>
       </c>
       <c r="H7" s="21">
-        <v>-1.4154579580275299E-9</v>
+        <v>-4.76663965044664E-5</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -4255,27 +4255,27 @@
         <v>200</v>
       </c>
       <c r="Y7" s="20">
-        <v>1.348747381556395E-3</v>
+        <v>0.39012343692375795</v>
       </c>
       <c r="Z7" s="20">
-        <v>-6.6081595942310001E-3</v>
+        <v>-0.459996016541806</v>
       </c>
       <c r="AA7" s="20">
-        <v>2.7937661256342299E-8</v>
+        <v>2.0410107431561801E-5</v>
       </c>
       <c r="AB7" s="20">
-        <v>-1.33461790304268E-8</v>
+        <v>-3.9342847907073503E-5</v>
       </c>
       <c r="AC7" s="21">
-        <v>-1.4154579580275299E-9</v>
+        <v>-4.76663965044664E-5</v>
       </c>
       <c r="AD7" s="25">
         <f t="array" ref="AD7">MAX(ABS(Y7:AC7))</f>
-        <v>6.6081595942310001E-3</v>
+        <v>0.459996016541806</v>
       </c>
       <c r="AE7" s="25">
         <f t="array" ref="AE7">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y7:$AC7),0))</f>
-        <v>2.7937661256342299E-8</v>
+        <v>4.76663965044664E-5</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -4286,19 +4286,19 @@
         <v>400</v>
       </c>
       <c r="D8" s="20">
-        <v>7.5693409509454607E-2</v>
+        <v>0.50176545481108903</v>
       </c>
       <c r="E8" s="20">
-        <v>0.92303530064188799</v>
+        <v>0.49652958491764299</v>
       </c>
       <c r="F8" s="20">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="G8" s="20">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="H8" s="21">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4321,27 +4321,27 @@
         <v>400</v>
       </c>
       <c r="Y8" s="20">
-        <v>2.2170950945460399E-4</v>
+        <v>0.426293754811089</v>
       </c>
       <c r="Z8" s="20">
-        <v>-1.4926993581120263E-3</v>
+        <v>-0.42799841508235703</v>
       </c>
       <c r="AA8" s="20">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="AB8" s="20">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="AC8" s="21">
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
       <c r="AD8" s="25">
         <f t="array" ref="AD8">MAX(ABS(Y8:AC8))</f>
-        <v>1.4926993581120263E-3</v>
+        <v>0.42799841508235703</v>
       </c>
       <c r="AE8" s="25">
         <f t="array" ref="AE8">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y8:$AC8),0))</f>
-        <v>5.7484766372765904E-12</v>
+        <v>2.1343365431027301E-11</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -4352,19 +4352,19 @@
         <v>400</v>
       </c>
       <c r="D9" s="20">
-        <v>7.5992367155662696E-2</v>
+        <v>0.50166916665714401</v>
       </c>
       <c r="E9" s="20">
-        <v>0.922829431495097</v>
+        <v>0.496464802208964</v>
       </c>
       <c r="F9" s="20">
-        <v>-1.5121830792196001E-9</v>
+        <v>1.1188662934728801E-10</v>
       </c>
       <c r="G9" s="20">
-        <v>-1.5121830792196001E-9</v>
+        <v>1.9757271171576599E-10</v>
       </c>
       <c r="H9" s="21">
-        <v>-1.5121830792196001E-9</v>
+        <v>4.1663017646078798E-10</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4387,27 +4387,27 @@
         <v>400</v>
       </c>
       <c r="Y9" s="20">
-        <v>5.206671556626935E-4</v>
+        <v>0.42619746665714398</v>
       </c>
       <c r="Z9" s="20">
-        <v>-1.6985685049030197E-3</v>
+        <v>-0.42806319779103602</v>
       </c>
       <c r="AA9" s="20">
-        <v>-1.5121830792196001E-9</v>
+        <v>1.1188662934728801E-10</v>
       </c>
       <c r="AB9" s="20">
-        <v>-1.5121830792196001E-9</v>
+        <v>1.9757271171576599E-10</v>
       </c>
       <c r="AC9" s="21">
-        <v>-1.5121830792196001E-9</v>
+        <v>4.1663017646078798E-10</v>
       </c>
       <c r="AD9" s="25">
         <f t="array" ref="AD9">MAX(ABS(Y9:AC9))</f>
-        <v>1.6985685049030197E-3</v>
+        <v>0.42806319779103602</v>
       </c>
       <c r="AE9" s="25">
         <f t="array" ref="AE9">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y9:$AC9),0))</f>
-        <v>1.5121830792196001E-9</v>
+        <v>4.1663017646078798E-10</v>
       </c>
     </row>
     <row r="10" spans="1:40" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4418,19 +4418,19 @@
         <v>800</v>
       </c>
       <c r="D10" s="39">
-        <v>7.5592437417003305E-2</v>
+        <v>0.50083453740408501</v>
       </c>
       <c r="E10" s="39">
-        <v>0.92390127952248302</v>
+        <v>0.49858393673586998</v>
       </c>
       <c r="F10" s="39">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="G10" s="39">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="H10" s="40">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
@@ -4453,27 +4453,27 @@
         <v>800</v>
       </c>
       <c r="Y10" s="39">
-        <v>1.2073741700330265E-4</v>
+        <v>0.42536283740408498</v>
       </c>
       <c r="Z10" s="39">
-        <v>-6.2672047751699544E-4</v>
+        <v>-0.42594406326413004</v>
       </c>
       <c r="AA10" s="39">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="AB10" s="39">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="AC10" s="40">
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="AD10" s="42">
         <f t="array" ref="AD10">MAX(ABS(Y10:AC10))</f>
-        <v>6.2672047751699544E-4</v>
+        <v>0.42594406326413004</v>
       </c>
       <c r="AE10" s="42">
         <f t="array" ref="AE10">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y10:$AC10),0))</f>
-        <v>1.25997092072913E-11</v>
+        <v>7.27034504236163E-12</v>
       </c>
       <c r="AF10" s="43"/>
       <c r="AM10" s="43"/>
@@ -4487,19 +4487,19 @@
         <v>800</v>
       </c>
       <c r="D11" s="20">
-        <v>7.5760164933455595E-2</v>
+        <v>0.498992028153395</v>
       </c>
       <c r="E11" s="20">
-        <v>0.92368695523845001</v>
+        <v>0.49939971562794899</v>
       </c>
       <c r="F11" s="20">
-        <v>-3.2998535347152299E-9</v>
+        <v>-3.0979261398993699E-6</v>
       </c>
       <c r="G11" s="20">
-        <v>-3.2998535347152299E-9</v>
+        <v>-5.8865896393516397E-6</v>
       </c>
       <c r="H11" s="21">
-        <v>-3.2998535347152299E-9</v>
+        <v>-2.92891975890727E-6</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -4522,27 +4522,27 @@
         <v>800</v>
       </c>
       <c r="Y11" s="20">
-        <v>2.8846493345559276E-4</v>
+        <v>0.42352032815339502</v>
       </c>
       <c r="Z11" s="20">
-        <v>-8.4104476155000274E-4</v>
+        <v>-0.42512828437205102</v>
       </c>
       <c r="AA11" s="20">
-        <v>-3.2998535347152299E-9</v>
+        <v>-3.0979261398993699E-6</v>
       </c>
       <c r="AB11" s="20">
-        <v>-3.2998535347152299E-9</v>
+        <v>-5.8865896393516397E-6</v>
       </c>
       <c r="AC11" s="21">
-        <v>-3.2998535347152299E-9</v>
+        <v>-2.92891975890727E-6</v>
       </c>
       <c r="AD11" s="25">
         <f t="array" ref="AD11">MAX(ABS(Y11:AC11))</f>
-        <v>8.4104476155000274E-4</v>
+        <v>0.42512828437205102</v>
       </c>
       <c r="AE11" s="25">
         <f t="array" ref="AE11">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y11:$AC11),0))</f>
-        <v>3.2998535347152299E-9</v>
+        <v>5.8865896393516397E-6</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -4553,19 +4553,19 @@
         <v>1600</v>
       </c>
       <c r="D12" s="20">
-        <v>7.5446438626921894E-2</v>
+        <v>-2.2777765644547698E-2</v>
       </c>
       <c r="E12" s="20">
-        <v>0.90968025925361595</v>
+        <v>2.63467733786268</v>
       </c>
       <c r="F12" s="20">
-        <v>1.15066129705472E-4</v>
+        <v>-3.1152408024714599E-4</v>
       </c>
       <c r="G12" s="20">
-        <v>5.8315343453775897E-5</v>
+        <v>-4.6716230654353797E-4</v>
       </c>
       <c r="H12" s="21">
-        <v>7.2846878203142003E-5</v>
+        <v>-4.1043341954494201E-4</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -4588,27 +4588,27 @@
         <v>1600</v>
       </c>
       <c r="Y12" s="20">
-        <v>-2.5261373078108718E-5</v>
+        <v>-9.8249465644547701E-2</v>
       </c>
       <c r="Z12" s="20">
-        <v>-1.4847740746384064E-2</v>
+        <v>1.71014933786268</v>
       </c>
       <c r="AA12" s="20">
-        <v>1.15066129705472E-4</v>
+        <v>-3.1152408024714599E-4</v>
       </c>
       <c r="AB12" s="20">
-        <v>5.8315343453775897E-5</v>
+        <v>-4.6716230654353797E-4</v>
       </c>
       <c r="AC12" s="21">
-        <v>7.2846878203142003E-5</v>
+        <v>-4.1043341954494201E-4</v>
       </c>
       <c r="AD12" s="25">
         <f t="array" ref="AD12">MAX(ABS(Y12:AC12))</f>
-        <v>1.4847740746384064E-2</v>
+        <v>1.71014933786268</v>
       </c>
       <c r="AE12" s="25">
         <f t="array" ref="AE12">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y12:$AC12),0))</f>
-        <v>1.15066129705472E-4</v>
+        <v>4.6716230654353797E-4</v>
       </c>
     </row>
     <row r="13" spans="1:40" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4619,19 +4619,19 @@
         <v>1600</v>
       </c>
       <c r="D13" s="67">
-        <v>0.35993359157190202</v>
+        <v>0.47003783553005801</v>
       </c>
       <c r="E13" s="67">
-        <v>0.34917505177029901</v>
+        <v>0.50912617175822195</v>
       </c>
       <c r="F13" s="67">
-        <v>-1.0461978271067E-3</v>
+        <v>-6.5506322041577201E-3</v>
       </c>
       <c r="G13" s="67">
-        <v>-1.01615870183224E-3</v>
+        <v>1.056033079088E-2</v>
       </c>
       <c r="H13" s="68">
-        <v>-1.0410243555181501E-3</v>
+        <v>8.7128350684926095E-3</v>
       </c>
       <c r="I13" s="69"/>
       <c r="J13" s="69"/>
@@ -4654,27 +4654,27 @@
         <v>1600</v>
       </c>
       <c r="Y13" s="67">
-        <v>0.28446189157190205</v>
+        <v>0.39456613553005804</v>
       </c>
       <c r="Z13" s="67">
-        <v>-0.57535294822970107</v>
+        <v>-0.41540182824177807</v>
       </c>
       <c r="AA13" s="67">
-        <v>-1.0461978271067E-3</v>
+        <v>-6.5506322041577201E-3</v>
       </c>
       <c r="AB13" s="67">
-        <v>-1.01615870183224E-3</v>
+        <v>1.056033079088E-2</v>
       </c>
       <c r="AC13" s="68">
-        <v>-1.0410243555181501E-3</v>
+        <v>8.7128350684926095E-3</v>
       </c>
       <c r="AD13" s="70">
         <f t="array" ref="AD13">MAX(ABS(Y13:AC13))</f>
-        <v>0.57535294822970107</v>
+        <v>0.41540182824177807</v>
       </c>
       <c r="AE13" s="70">
         <f t="array" ref="AE13">MAX(IF($Y$2:$AC$2&lt;$AE$2,ABS($Y13:$AC13),0))</f>
-        <v>1.0461978271067E-3</v>
+        <v>1.056033079088E-2</v>
       </c>
       <c r="AF13" s="13"/>
       <c r="AM13" s="13"/>
@@ -4689,12 +4689,10 @@
         <v>6</v>
       </c>
       <c r="D15" s="29">
-        <f>D2</f>
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="29">
-        <f>E2</f>
-        <v>0.92452800000000002</v>
+        <v>1</v>
       </c>
       <c r="F15" s="29">
         <f>F2</f>
@@ -4730,10 +4728,10 @@
         <v>Exact</v>
       </c>
       <c r="Y15" s="29">
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="Z15" s="29">
-        <v>0.92452800000000002</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="29">
         <v>0</v>
@@ -4821,19 +4819,19 @@
         <v>100</v>
       </c>
       <c r="D17" s="39">
-        <v>1</v>
+        <v>0.56470158890280797</v>
       </c>
       <c r="E17" s="39">
-        <v>0.49999738393896398</v>
+        <v>0.27499870162785001</v>
       </c>
       <c r="F17" s="39">
-        <v>0.49999738393896398</v>
+        <v>5.01995211680206E-4</v>
       </c>
       <c r="G17" s="39">
-        <v>0.49999738393896398</v>
+        <v>2.70461658556971E-4</v>
       </c>
       <c r="H17" s="40">
-        <v>0.49999738393896398</v>
+        <v>2.4924612005329099E-4</v>
       </c>
       <c r="I17" s="36"/>
       <c r="J17" s="36"/>
@@ -4858,27 +4856,27 @@
       </c>
       <c r="Y17" s="39">
         <f t="array" ref="Y17:AC26">D17:H26-Y15:AC15</f>
-        <v>0.92452829999999997</v>
+        <v>6.4701588902807972E-2</v>
       </c>
       <c r="Z17" s="39">
-        <v>-0.42453061606103604</v>
+        <v>-0.72500129837214999</v>
       </c>
       <c r="AA17" s="39">
-        <v>0.49999738393896398</v>
+        <v>5.01995211680206E-4</v>
       </c>
       <c r="AB17" s="39">
-        <v>0.49999738393896398</v>
+        <v>2.70461658556971E-4</v>
       </c>
       <c r="AC17" s="40">
-        <v>0.49999738393896398</v>
+        <v>2.4924612005329099E-4</v>
       </c>
       <c r="AD17" s="42">
         <f t="array" ref="AD17">MAX(ABS(Y17:AC17))</f>
-        <v>0.92452829999999997</v>
+        <v>0.72500129837214999</v>
       </c>
       <c r="AE17" s="42">
         <f t="array" ref="AE17">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y17:$AC17),0))</f>
-        <v>0.49999738393896398</v>
+        <v>5.01995211680206E-4</v>
       </c>
       <c r="AG17" s="36"/>
       <c r="AH17" s="36"/>
@@ -4895,19 +4893,19 @@
         <v>100</v>
       </c>
       <c r="D18" s="39">
-        <v>0.99967082061740697</v>
+        <v>0.50427239079730202</v>
       </c>
       <c r="E18" s="39">
-        <v>3.23796200503741E-4</v>
+        <v>0.48663980807887203</v>
       </c>
       <c r="F18" s="39">
-        <v>8.2277383336696406E-8</v>
+        <v>2.5375096031797201E-8</v>
       </c>
       <c r="G18" s="39">
-        <v>1.03089121469813E-9</v>
+        <v>1.49915406686836E-9</v>
       </c>
       <c r="H18" s="40">
-        <v>2.8866653367227001E-11</v>
+        <v>6.82429853629997E-12</v>
       </c>
       <c r="I18" s="36"/>
       <c r="J18" s="36"/>
@@ -4930,27 +4928,27 @@
         <v>100</v>
       </c>
       <c r="Y18" s="39">
-        <v>0.92419912061740694</v>
+        <v>4.272390797302017E-3</v>
       </c>
       <c r="Z18" s="39">
-        <v>-0.9242042037994963</v>
+        <v>-0.51336019192112792</v>
       </c>
       <c r="AA18" s="39">
-        <v>8.2277383336696406E-8</v>
+        <v>2.5375096031797201E-8</v>
       </c>
       <c r="AB18" s="39">
-        <v>1.03089121469813E-9</v>
+        <v>1.49915406686836E-9</v>
       </c>
       <c r="AC18" s="40">
-        <v>2.8866653367227001E-11</v>
+        <v>6.82429853629997E-12</v>
       </c>
       <c r="AD18" s="42">
         <f t="array" ref="AD18">MAX(ABS(Y18:AC18))</f>
-        <v>0.9242042037994963</v>
+        <v>0.51336019192112792</v>
       </c>
       <c r="AE18" s="42">
         <f t="array" ref="AE18">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y18:$AC18),0))</f>
-        <v>8.2277383336696406E-8</v>
+        <v>2.5375096031797201E-8</v>
       </c>
       <c r="AG18" s="36"/>
       <c r="AH18" s="36"/>
@@ -4967,19 +4965,19 @@
         <v>200</v>
       </c>
       <c r="D19" s="39">
-        <v>0.999999999999999</v>
+        <v>0.50393398198211903</v>
       </c>
       <c r="E19" s="39">
-        <v>0.999999999999999</v>
+        <v>0.49315465029949501</v>
       </c>
       <c r="F19" s="39">
-        <v>0.999999999999999</v>
+        <v>1.4307375449696299E-10</v>
       </c>
       <c r="G19" s="39">
-        <v>0.999999999999999</v>
+        <v>-1.10117325995644E-11</v>
       </c>
       <c r="H19" s="40">
-        <v>0.999999999999999</v>
+        <v>-1.10117325995644E-11</v>
       </c>
       <c r="I19" s="36"/>
       <c r="J19" s="36"/>
@@ -5002,27 +5000,27 @@
         <v>200</v>
       </c>
       <c r="Y19" s="39">
-        <v>0.92452829999999897</v>
+        <v>3.9339819821190281E-3</v>
       </c>
       <c r="Z19" s="39">
-        <v>7.5471999999998984E-2</v>
+        <v>-0.50684534970050499</v>
       </c>
       <c r="AA19" s="39">
-        <v>0.999999999999999</v>
+        <v>1.4307375449696299E-10</v>
       </c>
       <c r="AB19" s="39">
-        <v>0.999999999999999</v>
+        <v>-1.10117325995644E-11</v>
       </c>
       <c r="AC19" s="40">
-        <v>0.999999999999999</v>
+        <v>-1.10117325995644E-11</v>
       </c>
       <c r="AD19" s="42">
         <f t="array" ref="AD19">MAX(ABS(Y19:AC19))</f>
-        <v>0.999999999999999</v>
+        <v>0.50684534970050499</v>
       </c>
       <c r="AE19" s="42">
         <f t="array" ref="AE19">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y19:$AC19),0))</f>
-        <v>0.999999999999999</v>
+        <v>1.4307375449696299E-10</v>
       </c>
       <c r="AG19" s="36"/>
       <c r="AH19" s="36"/>
@@ -5039,19 +5037,19 @@
         <v>200</v>
       </c>
       <c r="D20" s="39">
-        <v>0.99608042200770797</v>
+        <v>0.50291719374513</v>
       </c>
       <c r="E20" s="39">
-        <v>3.62771731291306E-3</v>
+        <v>0.49258856006273399</v>
       </c>
       <c r="F20" s="39">
-        <v>2.8855660896845501E-4</v>
+        <v>-6.4792096819447403E-11</v>
       </c>
       <c r="G20" s="39">
-        <v>4.0982333173153297E-6</v>
+        <v>-2.0445032981720601E-11</v>
       </c>
       <c r="H20" s="40">
-        <v>-4.3609625023996798E-7</v>
+        <v>-2.0445032981720601E-11</v>
       </c>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
@@ -5074,27 +5072,27 @@
         <v>200</v>
       </c>
       <c r="Y20" s="39">
-        <v>0.92060872200770794</v>
+        <v>2.9171937451299979E-3</v>
       </c>
       <c r="Z20" s="39">
-        <v>-0.9209002826870869</v>
+        <v>-0.50741143993726601</v>
       </c>
       <c r="AA20" s="39">
-        <v>2.8855660896845501E-4</v>
+        <v>-6.4792096819447403E-11</v>
       </c>
       <c r="AB20" s="39">
-        <v>4.0982333173153297E-6</v>
+        <v>-2.0445032981720601E-11</v>
       </c>
       <c r="AC20" s="40">
-        <v>-4.3609625023996798E-7</v>
+        <v>-2.0445032981720601E-11</v>
       </c>
       <c r="AD20" s="42">
         <f t="array" ref="AD20">MAX(ABS(Y20:AC20))</f>
-        <v>0.9209002826870869</v>
+        <v>0.50741143993726601</v>
       </c>
       <c r="AE20" s="42">
         <f t="array" ref="AE20">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y20:$AC20),0))</f>
-        <v>2.8855660896845501E-4</v>
+        <v>6.4792096819447403E-11</v>
       </c>
       <c r="AG20" s="36"/>
       <c r="AH20" s="36"/>
@@ -5111,19 +5109,19 @@
         <v>400</v>
       </c>
       <c r="D21" s="39">
-        <v>1</v>
+        <v>0.75256883557614795</v>
       </c>
       <c r="E21" s="39">
-        <v>1</v>
+        <v>0.24663231052186099</v>
       </c>
       <c r="F21" s="39">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="G21" s="39">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="H21" s="40">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="I21" s="36"/>
       <c r="J21" s="36"/>
@@ -5146,27 +5144,27 @@
         <v>400</v>
       </c>
       <c r="Y21" s="39">
-        <v>0.92452829999999997</v>
+        <v>0.25256883557614795</v>
       </c>
       <c r="Z21" s="39">
-        <v>7.5471999999999984E-2</v>
+        <v>-0.75336768947813904</v>
       </c>
       <c r="AA21" s="39">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="AB21" s="39">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="AC21" s="40">
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="AD21" s="42">
         <f t="array" ref="AD21">MAX(ABS(Y21:AC21))</f>
-        <v>1</v>
+        <v>0.75336768947813904</v>
       </c>
       <c r="AE21" s="42">
         <f t="array" ref="AE21">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y21:$AC21),0))</f>
-        <v>1</v>
+        <v>5.7300599960380998E-13</v>
       </c>
       <c r="AG21" s="36"/>
       <c r="AH21" s="36"/>
@@ -5183,19 +5181,19 @@
         <v>400</v>
       </c>
       <c r="D22" s="39">
-        <v>0.99999957691097596</v>
+        <v>0.50168439469183601</v>
       </c>
       <c r="E22" s="39">
-        <v>0.50000041657043803</v>
+        <v>0.49637169538514098</v>
       </c>
       <c r="F22" s="39">
-        <v>0.50000000033606196</v>
+        <v>-2.3358628147654303E-10</v>
       </c>
       <c r="G22" s="39">
-        <v>0.50000000033606196</v>
+        <v>5.3468762479409501E-11</v>
       </c>
       <c r="H22" s="40">
-        <v>0.50000000033606196</v>
+        <v>5.3468762479409501E-11</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
@@ -5218,27 +5216,27 @@
         <v>400</v>
       </c>
       <c r="Y22" s="39">
-        <v>0.92452787691097593</v>
+        <v>1.6843946918360109E-3</v>
       </c>
       <c r="Z22" s="39">
-        <v>-0.42452758342956198</v>
+        <v>-0.50362830461485908</v>
       </c>
       <c r="AA22" s="39">
-        <v>0.50000000033606196</v>
+        <v>-2.3358628147654303E-10</v>
       </c>
       <c r="AB22" s="39">
-        <v>0.50000000033606196</v>
+        <v>5.3468762479409501E-11</v>
       </c>
       <c r="AC22" s="40">
-        <v>0.50000000033606196</v>
+        <v>5.3468762479409501E-11</v>
       </c>
       <c r="AD22" s="42">
         <f t="array" ref="AD22">MAX(ABS(Y22:AC22))</f>
-        <v>0.92452787691097593</v>
+        <v>0.50362830461485908</v>
       </c>
       <c r="AE22" s="42">
         <f t="array" ref="AE22">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y22:$AC22),0))</f>
-        <v>0.50000000033606196</v>
+        <v>2.3358628147654303E-10</v>
       </c>
       <c r="AG22" s="36"/>
       <c r="AH22" s="36"/>
@@ -5255,19 +5253,19 @@
         <v>800</v>
       </c>
       <c r="D23" s="39">
-        <v>1</v>
+        <v>0.500864498518381</v>
       </c>
       <c r="E23" s="39">
-        <v>1</v>
+        <v>0.49851680198734499</v>
       </c>
       <c r="F23" s="39">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="G23" s="39">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="H23" s="40">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
@@ -5290,27 +5288,27 @@
         <v>800</v>
       </c>
       <c r="Y23" s="39">
-        <v>0.92452829999999997</v>
+        <v>8.6449851838099612E-4</v>
       </c>
       <c r="Z23" s="39">
-        <v>7.5471999999999984E-2</v>
+        <v>-0.50148319801265506</v>
       </c>
       <c r="AA23" s="39">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="AB23" s="39">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="AC23" s="40">
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="AD23" s="42">
         <f t="array" ref="AD23">MAX(ABS(Y23:AC23))</f>
-        <v>1</v>
+        <v>0.50148319801265506</v>
       </c>
       <c r="AE23" s="42">
         <f t="array" ref="AE23">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y23:$AC23),0))</f>
-        <v>1</v>
+        <v>6.8565929474979504E-12</v>
       </c>
       <c r="AG23" s="36"/>
       <c r="AH23" s="36"/>
@@ -5327,19 +5325,19 @@
         <v>800</v>
       </c>
       <c r="D24" s="39">
-        <v>0.999999999999999</v>
+        <v>0.75150952849997799</v>
       </c>
       <c r="E24" s="39">
-        <v>0.999999999999999</v>
+        <v>0.24811905456738201</v>
       </c>
       <c r="F24" s="39">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="G24" s="39">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="H24" s="40">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
@@ -5362,27 +5360,27 @@
         <v>800</v>
       </c>
       <c r="Y24" s="39">
-        <v>0.92452829999999897</v>
+        <v>0.25150952849997799</v>
       </c>
       <c r="Z24" s="39">
-        <v>7.5471999999998984E-2</v>
+        <v>-0.75188094543261796</v>
       </c>
       <c r="AA24" s="39">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="AB24" s="39">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="AC24" s="40">
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="AD24" s="42">
         <f t="array" ref="AD24">MAX(ABS(Y24:AC24))</f>
-        <v>0.999999999999999</v>
+        <v>0.75188094543261796</v>
       </c>
       <c r="AE24" s="42">
         <f t="array" ref="AE24">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y24:$AC24),0))</f>
-        <v>0.999999999999999</v>
+        <v>1.3910966412834799E-10</v>
       </c>
       <c r="AG24" s="36"/>
       <c r="AH24" s="36"/>
@@ -5434,10 +5432,10 @@
         <v>1600</v>
       </c>
       <c r="Y25" s="39">
-        <v>0.92452829999999897</v>
+        <v>0.499999999999999</v>
       </c>
       <c r="Z25" s="39">
-        <v>7.5471999999998984E-2</v>
+        <v>-9.9920072216264089E-16</v>
       </c>
       <c r="AA25" s="39">
         <v>0.999999999999999</v>
@@ -5471,19 +5469,19 @@
         <v>1600</v>
       </c>
       <c r="D26" s="62">
-        <v>0.82554123251690603</v>
+        <v>0.49761183842505502</v>
       </c>
       <c r="E26" s="62">
-        <v>0.71270246796455305</v>
+        <v>0.48943374776875997</v>
       </c>
       <c r="F26" s="62">
-        <v>0.71270246796455305</v>
+        <v>1.60379468405218E-6</v>
       </c>
       <c r="G26" s="62">
-        <v>0.71270246796455305</v>
+        <v>1.17583113995393E-6</v>
       </c>
       <c r="H26" s="63">
-        <v>0.36886711265335698</v>
+        <v>1.17583113995393E-6</v>
       </c>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
@@ -5506,27 +5504,27 @@
         <v>1600</v>
       </c>
       <c r="Y26" s="62">
-        <v>0.750069532516906</v>
+        <v>-2.3881615749449803E-3</v>
       </c>
       <c r="Z26" s="62">
-        <v>-0.21182553203544696</v>
+        <v>-0.51056625223123997</v>
       </c>
       <c r="AA26" s="62">
-        <v>0.71270246796455305</v>
+        <v>1.60379468405218E-6</v>
       </c>
       <c r="AB26" s="62">
-        <v>0.71270246796455305</v>
+        <v>1.17583113995393E-6</v>
       </c>
       <c r="AC26" s="63">
-        <v>0.36886711265335698</v>
+        <v>1.17583113995393E-6</v>
       </c>
       <c r="AD26" s="64">
         <f t="array" ref="AD26">MAX(ABS(Y26:AC26))</f>
-        <v>0.750069532516906</v>
+        <v>0.51056625223123997</v>
       </c>
       <c r="AE26" s="64">
         <f t="array" ref="AE26">MAX(IF(Y$15:AC$15&lt;$AE$15,ABS($Y26:$AC26),0))</f>
-        <v>0.71270246796455305</v>
+        <v>1.60379468405218E-6</v>
       </c>
       <c r="AG26" s="36"/>
       <c r="AH26" s="36"/>
@@ -5544,7 +5542,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="29">
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="29">
         <v>1</v>
@@ -5566,7 +5564,7 @@
         <v>Exact</v>
       </c>
       <c r="Y29" s="29">
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="Z29" s="29">
         <v>1</v>
@@ -5643,16 +5641,16 @@
         <v>100</v>
       </c>
       <c r="D31" s="20">
-        <v>7.7136027250608197E-2</v>
+        <v>0.566785397777536</v>
       </c>
       <c r="E31" s="20">
-        <v>1</v>
+        <v>0.815430079499052</v>
       </c>
       <c r="F31" s="20">
-        <v>1</v>
+        <v>0.81859571170900003</v>
       </c>
       <c r="G31" s="20">
-        <v>1</v>
+        <v>0.82189531259471704</v>
       </c>
       <c r="H31" s="21">
         <v>1</v>
@@ -5680,27 +5678,27 @@
       </c>
       <c r="Y31" s="20">
         <f t="array" ref="Y31:AC40">D31:H40-Y29:AC29</f>
-        <v>1.6643272506081941E-3</v>
+        <v>6.6785397777536004E-2</v>
       </c>
       <c r="Z31" s="20">
-        <v>0</v>
+        <v>-0.184569920500948</v>
       </c>
       <c r="AA31" s="20">
-        <v>0</v>
+        <v>-0.18140428829099997</v>
       </c>
       <c r="AB31" s="20">
-        <v>0</v>
+        <v>-0.17810468740528296</v>
       </c>
       <c r="AC31" s="21">
         <v>0</v>
       </c>
       <c r="AD31" s="25">
         <f t="array" ref="AD31">MAX(ABS(Y31:AC31))</f>
-        <v>1.6643272506081941E-3</v>
+        <v>0.184569920500948</v>
       </c>
       <c r="AE31" s="25">
         <f t="array" ref="AE31">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y31:$AC31),0))</f>
-        <v>0</v>
+        <v>0.184569920500948</v>
       </c>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.25">
@@ -5711,16 +5709,16 @@
         <v>100</v>
       </c>
       <c r="D32" s="20">
-        <v>3.9532334089099001E-2</v>
+        <v>0.50100371618402195</v>
       </c>
       <c r="E32" s="20">
-        <v>0.50012265506786502</v>
+        <v>0.999999406066715</v>
       </c>
       <c r="F32" s="20">
-        <v>0.50012274531806999</v>
+        <v>0.99999956740698503</v>
       </c>
       <c r="G32" s="20">
-        <v>0.50012276322123494</v>
+        <v>0.99999976403635604</v>
       </c>
       <c r="H32" s="21">
         <v>1</v>
@@ -5746,27 +5744,27 @@
         <v>100</v>
       </c>
       <c r="Y32" s="20">
-        <v>-3.5939365910901001E-2</v>
+        <v>1.0037161840219522E-3</v>
       </c>
       <c r="Z32" s="20">
-        <v>-0.49987734493213498</v>
+        <v>-5.9393328499801612E-7</v>
       </c>
       <c r="AA32" s="20">
-        <v>-0.49987725468193001</v>
+        <v>-4.3259301496512137E-7</v>
       </c>
       <c r="AB32" s="20">
-        <v>-0.49987723677876506</v>
+        <v>-2.3596364395750413E-7</v>
       </c>
       <c r="AC32" s="21">
         <v>0</v>
       </c>
       <c r="AD32" s="25">
         <f t="array" ref="AD32">MAX(ABS(Y32:AC32))</f>
-        <v>0.49987734493213498</v>
+        <v>1.0037161840219522E-3</v>
       </c>
       <c r="AE32" s="25">
         <f t="array" ref="AE32">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y32:$AC32),0))</f>
-        <v>0.49987734493213498</v>
+        <v>5.9393328499801612E-7</v>
       </c>
     </row>
     <row r="33" spans="2:38" x14ac:dyDescent="0.25">
@@ -5777,16 +5775,16 @@
         <v>200</v>
       </c>
       <c r="D33" s="20">
-        <v>7.7794435976047904E-2</v>
+        <v>0.50387272716312204</v>
       </c>
       <c r="E33" s="20">
-        <v>1</v>
+        <v>0.99999999994421296</v>
       </c>
       <c r="F33" s="20">
-        <v>1</v>
+        <v>1.0000000000499001</v>
       </c>
       <c r="G33" s="20">
-        <v>1</v>
+        <v>1.00000000001359</v>
       </c>
       <c r="H33" s="21">
         <v>1</v>
@@ -5812,27 +5810,27 @@
         <v>200</v>
       </c>
       <c r="Y33" s="20">
-        <v>2.3227359760479016E-3</v>
+        <v>3.8727271631220361E-3</v>
       </c>
       <c r="Z33" s="20">
-        <v>0</v>
+        <v>-5.5787041652877178E-11</v>
       </c>
       <c r="AA33" s="20">
-        <v>0</v>
+        <v>4.9900084064802286E-11</v>
       </c>
       <c r="AB33" s="20">
-        <v>0</v>
+        <v>1.3590017999831616E-11</v>
       </c>
       <c r="AC33" s="21">
         <v>0</v>
       </c>
       <c r="AD33" s="25">
         <f t="array" ref="AD33">MAX(ABS(Y33:AC33))</f>
-        <v>2.3227359760479016E-3</v>
+        <v>3.8727271631220361E-3</v>
       </c>
       <c r="AE33" s="25">
         <f t="array" ref="AE33">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y33:$AC33),0))</f>
-        <v>0</v>
+        <v>5.5787041652877178E-11</v>
       </c>
     </row>
     <row r="34" spans="2:38" x14ac:dyDescent="0.25">
@@ -5843,16 +5841,16 @@
         <v>200</v>
       </c>
       <c r="D34" s="20">
-        <v>7.6820447381556398E-2</v>
+        <v>0.46559513692375798</v>
       </c>
       <c r="E34" s="20">
-        <v>0.999999335944881</v>
+        <v>0.99987035240506905</v>
       </c>
       <c r="F34" s="20">
-        <v>0.99999957284394703</v>
+        <v>0.99985431080906495</v>
       </c>
       <c r="G34" s="20">
-        <v>0.99999983982513796</v>
+        <v>0.99991382330606005</v>
       </c>
       <c r="H34" s="21">
         <v>1</v>
@@ -5878,27 +5876,27 @@
         <v>200</v>
       </c>
       <c r="Y34" s="20">
-        <v>1.348747381556395E-3</v>
+        <v>-3.440486307624202E-2</v>
       </c>
       <c r="Z34" s="20">
-        <v>-6.6405511900402558E-7</v>
+        <v>-1.2964759493094835E-4</v>
       </c>
       <c r="AA34" s="20">
-        <v>-4.2715605297338755E-7</v>
+        <v>-1.4568919093504995E-4</v>
       </c>
       <c r="AB34" s="20">
-        <v>-1.6017486204056297E-7</v>
+        <v>-8.6176693939954419E-5</v>
       </c>
       <c r="AC34" s="21">
         <v>0</v>
       </c>
       <c r="AD34" s="25">
         <f t="array" ref="AD34">MAX(ABS(Y34:AC34))</f>
-        <v>1.348747381556395E-3</v>
+        <v>3.440486307624202E-2</v>
       </c>
       <c r="AE34" s="25">
         <f t="array" ref="AE34">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y34:$AC34),0))</f>
-        <v>6.6405511900402558E-7</v>
+        <v>1.4568919093504995E-4</v>
       </c>
     </row>
     <row r="35" spans="2:38" x14ac:dyDescent="0.25">
@@ -5909,10 +5907,10 @@
         <v>400</v>
       </c>
       <c r="D35" s="20">
-        <v>7.5693409509454607E-2</v>
+        <v>0.50176545481108903</v>
       </c>
       <c r="E35" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F35" s="20">
         <v>1</v>
@@ -5944,10 +5942,10 @@
         <v>400</v>
       </c>
       <c r="Y35" s="20">
-        <v>2.2170950945460399E-4</v>
+        <v>1.7654548110890289E-3</v>
       </c>
       <c r="Z35" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AA35" s="20">
         <v>0</v>
@@ -5960,11 +5958,11 @@
       </c>
       <c r="AD35" s="25">
         <f t="array" ref="AD35">MAX(ABS(Y35:AC35))</f>
-        <v>2.2170950945460399E-4</v>
+        <v>1.7654548110890289E-3</v>
       </c>
       <c r="AE35" s="25">
         <f t="array" ref="AE35">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y35:$AC35),0))</f>
-        <v>9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:38" x14ac:dyDescent="0.25">
@@ -5975,16 +5973,16 @@
         <v>400</v>
       </c>
       <c r="D36" s="20">
-        <v>7.5992367155662696E-2</v>
+        <v>0.50166916665714401</v>
       </c>
       <c r="E36" s="20">
-        <v>0.99999999998174105</v>
+        <v>0.99999999827028196</v>
       </c>
       <c r="F36" s="20">
-        <v>0.99999999998174105</v>
+        <v>0.99999999835527598</v>
       </c>
       <c r="G36" s="20">
-        <v>0.99999999998174205</v>
+        <v>0.99999999884543</v>
       </c>
       <c r="H36" s="21">
         <v>1</v>
@@ -6010,27 +6008,27 @@
         <v>400</v>
       </c>
       <c r="Y36" s="20">
-        <v>5.206671556626935E-4</v>
+        <v>1.6691666571440056E-3</v>
       </c>
       <c r="Z36" s="20">
-        <v>-1.8258949907590249E-11</v>
+        <v>-1.7297180354702846E-9</v>
       </c>
       <c r="AA36" s="20">
-        <v>-1.8258949907590249E-11</v>
+        <v>-1.644724023641686E-9</v>
       </c>
       <c r="AB36" s="20">
-        <v>-1.8257950706868087E-11</v>
+        <v>-1.1545699951653887E-9</v>
       </c>
       <c r="AC36" s="21">
         <v>0</v>
       </c>
       <c r="AD36" s="25">
         <f t="array" ref="AD36">MAX(ABS(Y36:AC36))</f>
-        <v>5.206671556626935E-4</v>
+        <v>1.6691666571440056E-3</v>
       </c>
       <c r="AE36" s="25">
         <f t="array" ref="AE36">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y36:$AC36),0))</f>
-        <v>1.8258949907590249E-11</v>
+        <v>1.7297180354702846E-9</v>
       </c>
     </row>
     <row r="37" spans="2:38" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6041,13 +6039,13 @@
         <v>800</v>
       </c>
       <c r="D37" s="52">
-        <v>7.5592437417003305E-2</v>
+        <v>0.50083453740408501</v>
       </c>
       <c r="E37" s="52">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F37" s="52">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G37" s="52">
         <v>1</v>
@@ -6076,13 +6074,13 @@
         <v>800</v>
       </c>
       <c r="Y37" s="52">
-        <v>1.2073741700330265E-4</v>
+        <v>8.3453740408501176E-4</v>
       </c>
       <c r="Z37" s="52">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AA37" s="52">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AB37" s="52">
         <v>0</v>
@@ -6092,11 +6090,11 @@
       </c>
       <c r="AD37" s="54">
         <f t="array" ref="AD37">MAX(ABS(Y37:AC37))</f>
-        <v>1.2073741700330265E-4</v>
+        <v>8.3453740408501176E-4</v>
       </c>
       <c r="AE37" s="54">
         <f t="array" ref="AE37">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y37:$AC37),0))</f>
-        <v>9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AG37" s="9"/>
       <c r="AH37" s="9"/>
@@ -6113,16 +6111,16 @@
         <v>800</v>
       </c>
       <c r="D38" s="20">
-        <v>7.5760164933455595E-2</v>
+        <v>0.498992028153395</v>
       </c>
       <c r="E38" s="20">
-        <v>0.999999999999999</v>
+        <v>1.0000141741822099</v>
       </c>
       <c r="F38" s="20">
-        <v>0.999999999999999</v>
+        <v>1.0000097249211499</v>
       </c>
       <c r="G38" s="20">
-        <v>0.999999999999999</v>
+        <v>0.99999852149614898</v>
       </c>
       <c r="H38" s="21">
         <v>1</v>
@@ -6148,27 +6146,27 @@
         <v>800</v>
       </c>
       <c r="Y38" s="20">
-        <v>2.8846493345559276E-4</v>
+        <v>-1.0079718466050047E-3</v>
       </c>
       <c r="Z38" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>1.4174182209947261E-5</v>
       </c>
       <c r="AA38" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>9.7249211499228494E-6</v>
       </c>
       <c r="AB38" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>-1.4785038510156667E-6</v>
       </c>
       <c r="AC38" s="21">
         <v>0</v>
       </c>
       <c r="AD38" s="25">
         <f t="array" ref="AD38">MAX(ABS(Y38:AC38))</f>
-        <v>2.8846493345559276E-4</v>
+        <v>1.0079718466050047E-3</v>
       </c>
       <c r="AE38" s="25">
         <f t="array" ref="AE38">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y38:$AC38),0))</f>
-        <v>9.9920072216264089E-16</v>
+        <v>1.4174182209947261E-5</v>
       </c>
     </row>
     <row r="39" spans="2:38" x14ac:dyDescent="0.25">
@@ -6179,16 +6177,16 @@
         <v>1600</v>
       </c>
       <c r="D39" s="20">
-        <v>7.5446438626921894E-2</v>
+        <v>-2.2777765644547698E-2</v>
       </c>
       <c r="E39" s="20">
-        <v>0.98710859694880804</v>
+        <v>0.95556237450112702</v>
       </c>
       <c r="F39" s="20">
-        <v>0.98921577545478701</v>
+        <v>0.96248660369341699</v>
       </c>
       <c r="G39" s="20">
-        <v>0.99245693097237697</v>
+        <v>0.97466763320571304</v>
       </c>
       <c r="H39" s="21">
         <v>1</v>
@@ -6214,27 +6212,27 @@
         <v>1600</v>
       </c>
       <c r="Y39" s="20">
-        <v>-2.5261373078108718E-5</v>
+        <v>-0.5227777656445477</v>
       </c>
       <c r="Z39" s="20">
-        <v>-1.2891403051191963E-2</v>
+        <v>-4.4437625498872979E-2</v>
       </c>
       <c r="AA39" s="20">
-        <v>-1.0784224545212995E-2</v>
+        <v>-3.7513396306583013E-2</v>
       </c>
       <c r="AB39" s="20">
-        <v>-7.5430690276230283E-3</v>
+        <v>-2.5332366794286965E-2</v>
       </c>
       <c r="AC39" s="21">
         <v>0</v>
       </c>
       <c r="AD39" s="25">
         <f t="array" ref="AD39">MAX(ABS(Y39:AC39))</f>
-        <v>1.2891403051191963E-2</v>
+        <v>0.5227777656445477</v>
       </c>
       <c r="AE39" s="25">
         <f t="array" ref="AE39">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y39:$AC39),0))</f>
-        <v>1.2891403051191963E-2</v>
+        <v>4.4437625498872979E-2</v>
       </c>
     </row>
     <row r="40" spans="2:38" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6245,16 +6243,16 @@
         <v>1600</v>
       </c>
       <c r="D40" s="67">
-        <v>0.35993359157190202</v>
+        <v>0.47003783553005801</v>
       </c>
       <c r="E40" s="67">
-        <v>0.98570559080368403</v>
+        <v>0.97728401626503703</v>
       </c>
       <c r="F40" s="67">
-        <v>1.01672852339541</v>
+        <v>0.98158773693677803</v>
       </c>
       <c r="G40" s="67">
-        <v>1.0262240189263301</v>
+        <v>1.0010282609998999</v>
       </c>
       <c r="H40" s="68">
         <v>1</v>
@@ -6280,27 +6278,27 @@
         <v>1600</v>
       </c>
       <c r="Y40" s="67">
-        <v>0.28446189157190205</v>
+        <v>-2.9962164469941988E-2</v>
       </c>
       <c r="Z40" s="67">
-        <v>-1.4294409196315971E-2</v>
+        <v>-2.2715983734962975E-2</v>
       </c>
       <c r="AA40" s="67">
-        <v>1.6728523395409978E-2</v>
+        <v>-1.8412263063221967E-2</v>
       </c>
       <c r="AB40" s="67">
-        <v>2.6224018926330084E-2</v>
+        <v>1.0282609998999437E-3</v>
       </c>
       <c r="AC40" s="68">
         <v>0</v>
       </c>
       <c r="AD40" s="70">
         <f t="array" ref="AD40">MAX(ABS(Y40:AC40))</f>
-        <v>0.28446189157190205</v>
+        <v>2.9962164469941988E-2</v>
       </c>
       <c r="AE40" s="70">
         <f t="array" ref="AE40">MAX(IF($Y$29:$AC$29&gt;1-$AE$29,ABS($Y40:$AC40),0))</f>
-        <v>2.6224018926330084E-2</v>
+        <v>2.2715983734962975E-2</v>
       </c>
       <c r="AG40" s="14"/>
       <c r="AH40" s="14"/>
@@ -6319,7 +6317,7 @@
       </c>
       <c r="D42" s="29">
         <f>D29</f>
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="29">
         <f>E29</f>
@@ -6359,7 +6357,7 @@
         <v>Exact</v>
       </c>
       <c r="Y42" s="29">
-        <v>7.5471700000000003E-2</v>
+        <v>0.5</v>
       </c>
       <c r="Z42" s="29">
         <v>1</v>
@@ -6450,16 +6448,16 @@
         <v>100</v>
       </c>
       <c r="D44" s="20">
-        <v>1</v>
+        <v>0.56470158890280797</v>
       </c>
       <c r="E44" s="20">
-        <v>1</v>
+        <v>0.96440256127507695</v>
       </c>
       <c r="F44" s="20">
-        <v>1</v>
+        <v>0.98571312024775504</v>
       </c>
       <c r="G44" s="20">
-        <v>1</v>
+        <v>0.99635236701739505</v>
       </c>
       <c r="H44" s="21">
         <v>1</v>
@@ -6473,27 +6471,27 @@
       </c>
       <c r="Y44" s="20">
         <f t="array" ref="Y44:AC53">D44:H53-Y42:AC42</f>
-        <v>0.92452829999999997</v>
+        <v>6.4701588902807972E-2</v>
       </c>
       <c r="Z44" s="20">
-        <v>0</v>
+        <v>-3.5597438724923047E-2</v>
       </c>
       <c r="AA44" s="20">
-        <v>0</v>
+        <v>-1.4286879752244963E-2</v>
       </c>
       <c r="AB44" s="20">
-        <v>0</v>
+        <v>-3.6476329826049536E-3</v>
       </c>
       <c r="AC44" s="21">
         <v>0</v>
       </c>
       <c r="AD44" s="25">
         <f t="array" ref="AD44">MAX(ABS(Y44:AC44))</f>
-        <v>0.92452829999999997</v>
+        <v>6.4701588902807972E-2</v>
       </c>
       <c r="AE44" s="25">
         <f t="array" ref="AE44">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y44:$AC44),0))</f>
-        <v>0</v>
+        <v>3.5597438724923047E-2</v>
       </c>
     </row>
     <row r="45" spans="2:38" x14ac:dyDescent="0.25">
@@ -6504,16 +6502,16 @@
         <v>100</v>
       </c>
       <c r="D45" s="20">
-        <v>0.99967082061740697</v>
+        <v>0.50427239079730202</v>
       </c>
       <c r="E45" s="20">
-        <v>0.99999991647048303</v>
+        <v>0.99999967681915303</v>
       </c>
       <c r="F45" s="20">
-        <v>0.99999999918704596</v>
+        <v>1.00000000119101</v>
       </c>
       <c r="G45" s="20">
-        <v>0.99999999999987399</v>
+        <v>1</v>
       </c>
       <c r="H45" s="21">
         <v>1</v>
@@ -6525,27 +6523,27 @@
         <v>100</v>
       </c>
       <c r="Y45" s="20">
-        <v>0.92419912061740694</v>
+        <v>4.272390797302017E-3</v>
       </c>
       <c r="Z45" s="20">
-        <v>-8.3529516969882422E-8</v>
+        <v>-3.2318084697280369E-7</v>
       </c>
       <c r="AA45" s="20">
-        <v>-8.1295403742132066E-10</v>
+        <v>1.1910099573242405E-9</v>
       </c>
       <c r="AB45" s="20">
-        <v>-1.2601031329495527E-13</v>
+        <v>0</v>
       </c>
       <c r="AC45" s="21">
         <v>0</v>
       </c>
       <c r="AD45" s="25">
         <f t="array" ref="AD45">MAX(ABS(Y45:AC45))</f>
-        <v>0.92419912061740694</v>
+        <v>4.272390797302017E-3</v>
       </c>
       <c r="AE45" s="25">
         <f t="array" ref="AE45">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y45:$AC45),0))</f>
-        <v>8.3529516969882422E-8</v>
+        <v>3.2318084697280369E-7</v>
       </c>
     </row>
     <row r="46" spans="2:38" x14ac:dyDescent="0.25">
@@ -6556,13 +6554,13 @@
         <v>200</v>
       </c>
       <c r="D46" s="20">
-        <v>0.999999999999999</v>
+        <v>0.50393398198211903</v>
       </c>
       <c r="E46" s="20">
-        <v>0.999999999999999</v>
+        <v>0.99999999886449698</v>
       </c>
       <c r="F46" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G46" s="20">
         <v>1</v>
@@ -6577,13 +6575,13 @@
         <v>200</v>
       </c>
       <c r="Y46" s="20">
-        <v>0.92452829999999897</v>
+        <v>3.9339819821190281E-3</v>
       </c>
       <c r="Z46" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>-1.1355030249404763E-9</v>
       </c>
       <c r="AA46" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AB46" s="20">
         <v>0</v>
@@ -6593,11 +6591,11 @@
       </c>
       <c r="AD46" s="25">
         <f t="array" ref="AD46">MAX(ABS(Y46:AC46))</f>
-        <v>0.92452829999999897</v>
+        <v>3.9339819821190281E-3</v>
       </c>
       <c r="AE46" s="25">
         <f t="array" ref="AE46">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y46:$AC46),0))</f>
-        <v>9.9920072216264089E-16</v>
+        <v>1.1355030249404763E-9</v>
       </c>
     </row>
     <row r="47" spans="2:38" x14ac:dyDescent="0.25">
@@ -6608,16 +6606,16 @@
         <v>200</v>
       </c>
       <c r="D47" s="20">
-        <v>0.99608042200770797</v>
+        <v>0.50291719374513</v>
       </c>
       <c r="E47" s="20">
-        <v>0.99970611964239697</v>
+        <v>0.99999999916693705</v>
       </c>
       <c r="F47" s="20">
-        <v>0.99999677692910105</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="G47" s="20">
-        <v>0.99999999999809397</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="H47" s="21">
         <v>1</v>
@@ -6629,27 +6627,27 @@
         <v>200</v>
       </c>
       <c r="Y47" s="20">
-        <v>0.92060872200770794</v>
+        <v>2.9171937451299979E-3</v>
       </c>
       <c r="Z47" s="20">
-        <v>-2.9388035760302689E-4</v>
+        <v>-8.3306295195484381E-10</v>
       </c>
       <c r="AA47" s="20">
-        <v>-3.2230708989500201E-6</v>
+        <v>-9.9920072216264089E-16</v>
       </c>
       <c r="AB47" s="20">
-        <v>-1.9060308886764687E-12</v>
+        <v>-9.9920072216264089E-16</v>
       </c>
       <c r="AC47" s="21">
         <v>0</v>
       </c>
       <c r="AD47" s="25">
         <f t="array" ref="AD47">MAX(ABS(Y47:AC47))</f>
-        <v>0.92060872200770794</v>
+        <v>2.9171937451299979E-3</v>
       </c>
       <c r="AE47" s="25">
         <f t="array" ref="AE47">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y47:$AC47),0))</f>
-        <v>2.9388035760302689E-4</v>
+        <v>8.3306295195484381E-10</v>
       </c>
     </row>
     <row r="48" spans="2:38" x14ac:dyDescent="0.25">
@@ -6660,7 +6658,7 @@
         <v>400</v>
       </c>
       <c r="D48" s="20">
-        <v>1</v>
+        <v>0.75256883557614795</v>
       </c>
       <c r="E48" s="20">
         <v>1</v>
@@ -6681,7 +6679,7 @@
         <v>400</v>
       </c>
       <c r="Y48" s="20">
-        <v>0.92452829999999997</v>
+        <v>0.25256883557614795</v>
       </c>
       <c r="Z48" s="20">
         <v>0</v>
@@ -6697,7 +6695,7 @@
       </c>
       <c r="AD48" s="25">
         <f t="array" ref="AD48">MAX(ABS(Y48:AC48))</f>
-        <v>0.92452829999999997</v>
+        <v>0.25256883557614795</v>
       </c>
       <c r="AE48" s="25">
         <f t="array" ref="AE48">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y48:$AC48),0))</f>
@@ -6712,16 +6710,16 @@
         <v>400</v>
       </c>
       <c r="D49" s="20">
-        <v>0.99999957691097596</v>
+        <v>0.50168439469183601</v>
       </c>
       <c r="E49" s="20">
-        <v>1.0000000001246501</v>
+        <v>0.99999999823044206</v>
       </c>
       <c r="F49" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G49" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="H49" s="21">
         <v>1</v>
@@ -6733,27 +6731,27 @@
         <v>400</v>
       </c>
       <c r="Y49" s="20">
-        <v>0.92452787691097593</v>
+        <v>1.6843946918360109E-3</v>
       </c>
       <c r="Z49" s="20">
-        <v>1.2465006804518453E-10</v>
+        <v>-1.7695579446197485E-9</v>
       </c>
       <c r="AA49" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AB49" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="21">
         <v>0</v>
       </c>
       <c r="AD49" s="25">
         <f t="array" ref="AD49">MAX(ABS(Y49:AC49))</f>
-        <v>0.92452787691097593</v>
+        <v>1.6843946918360109E-3</v>
       </c>
       <c r="AE49" s="25">
         <f t="array" ref="AE49">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y49:$AC49),0))</f>
-        <v>1.2465006804518453E-10</v>
+        <v>1.7695579446197485E-9</v>
       </c>
     </row>
     <row r="50" spans="2:38" x14ac:dyDescent="0.25">
@@ -6764,7 +6762,7 @@
         <v>800</v>
       </c>
       <c r="D50" s="20">
-        <v>1</v>
+        <v>0.500864498518381</v>
       </c>
       <c r="E50" s="20">
         <v>1</v>
@@ -6785,7 +6783,7 @@
         <v>800</v>
       </c>
       <c r="Y50" s="20">
-        <v>0.92452829999999997</v>
+        <v>8.6449851838099612E-4</v>
       </c>
       <c r="Z50" s="20">
         <v>0</v>
@@ -6801,7 +6799,7 @@
       </c>
       <c r="AD50" s="25">
         <f t="array" ref="AD50">MAX(ABS(Y50:AC50))</f>
-        <v>0.92452829999999997</v>
+        <v>8.6449851838099612E-4</v>
       </c>
       <c r="AE50" s="25">
         <f t="array" ref="AE50">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y50:$AC50),0))</f>
@@ -6816,16 +6814,16 @@
         <v>800</v>
       </c>
       <c r="D51" s="20">
-        <v>0.999999999999999</v>
+        <v>0.75150952849997799</v>
       </c>
       <c r="E51" s="20">
         <v>0.999999999999999</v>
       </c>
       <c r="F51" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G51" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="H51" s="21">
         <v>1</v>
@@ -6837,23 +6835,23 @@
         <v>800</v>
       </c>
       <c r="Y51" s="20">
-        <v>0.92452829999999897</v>
+        <v>0.25150952849997799</v>
       </c>
       <c r="Z51" s="20">
         <v>-9.9920072216264089E-16</v>
       </c>
       <c r="AA51" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AB51" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="21">
         <v>0</v>
       </c>
       <c r="AD51" s="25">
         <f t="array" ref="AD51">MAX(ABS(Y51:AC51))</f>
-        <v>0.92452829999999897</v>
+        <v>0.25150952849997799</v>
       </c>
       <c r="AE51" s="25">
         <f t="array" ref="AE51">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y51:$AC51),0))</f>
@@ -6871,7 +6869,7 @@
         <v>0.999999999999999</v>
       </c>
       <c r="E52" s="20">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F52" s="20">
         <v>1</v>
@@ -6889,10 +6887,10 @@
         <v>1600</v>
       </c>
       <c r="Y52" s="20">
-        <v>0.92452829999999897</v>
+        <v>0.499999999999999</v>
       </c>
       <c r="Z52" s="20">
-        <v>-9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="20">
         <v>0</v>
@@ -6905,11 +6903,11 @@
       </c>
       <c r="AD52" s="25">
         <f t="array" ref="AD52">MAX(ABS(Y52:AC52))</f>
-        <v>0.92452829999999897</v>
+        <v>0.499999999999999</v>
       </c>
       <c r="AE52" s="25">
         <f t="array" ref="AE52">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y52:$AC52),0))</f>
-        <v>9.9920072216264089E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:38" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6920,16 +6918,16 @@
         <v>1600</v>
       </c>
       <c r="D53" s="67">
-        <v>0.82554123251690603</v>
+        <v>0.49761183842505502</v>
       </c>
       <c r="E53" s="67">
-        <v>0.849628654193195</v>
+        <v>0.99996320111905701</v>
       </c>
       <c r="F53" s="67">
-        <v>0.85124741317555697</v>
+        <v>1</v>
       </c>
       <c r="G53" s="67">
-        <v>0.84263250158823499</v>
+        <v>1</v>
       </c>
       <c r="H53" s="68">
         <v>1</v>
@@ -6955,27 +6953,27 @@
         <v>1600</v>
       </c>
       <c r="Y53" s="67">
-        <v>0.750069532516906</v>
+        <v>-2.3881615749449803E-3</v>
       </c>
       <c r="Z53" s="67">
-        <v>-0.150371345806805</v>
+        <v>-3.6798880942989776E-5</v>
       </c>
       <c r="AA53" s="67">
-        <v>-0.14875258682444303</v>
+        <v>0</v>
       </c>
       <c r="AB53" s="67">
-        <v>-0.15736749841176501</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="68">
         <v>0</v>
       </c>
       <c r="AD53" s="70">
         <f t="array" ref="AD53">MAX(ABS(Y53:AC53))</f>
-        <v>0.750069532516906</v>
+        <v>2.3881615749449803E-3</v>
       </c>
       <c r="AE53" s="70">
         <f t="array" ref="AE53">MAX(IF($Y$42:$AC$42&gt;1-$AE$42,ABS($Y53:$AC53),0))</f>
-        <v>0.15736749841176501</v>
+        <v>3.6798880942989776E-5</v>
       </c>
       <c r="AG53" s="14"/>
       <c r="AH53" s="14"/>
@@ -6993,8 +6991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="AD37" sqref="AD37"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="AD40" sqref="AD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>